<commit_message>
change data output format
</commit_message>
<xml_diff>
--- a/Interannual_metrics_conversion.xlsx
+++ b/Interannual_metrics_conversion.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noellepatterson/apps/Other/Climate_change_research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A244D5A-994D-CB43-A651-A7D7867D2C80}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D331257-78A9-9A4B-9AB7-2E860FD92B19}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1260" yWindow="1640" windowWidth="15900" windowHeight="14700" xr2:uid="{ADBF414B-E432-A949-8C08-2739CE937D51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -451,7 +451,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -828,8 +828,8 @@
         <v>29.538999999999994</v>
       </c>
       <c r="H21">
-        <f>G21/100*0.4+0.4</f>
-        <v>0.51815600000000006</v>
+        <f>G21/100*0.2+0.2</f>
+        <v>0.25907800000000003</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -855,8 +855,8 @@
         <v>53.21</v>
       </c>
       <c r="H22">
-        <f>G22/100*0.4+0.4</f>
-        <v>0.61284000000000005</v>
+        <f>G22/100*0.2+0.2</f>
+        <v>0.30642000000000003</v>
       </c>
     </row>
     <row r="23" spans="1:8">

</xml_diff>

<commit_message>
automate precip script through scenario runs
</commit_message>
<xml_diff>
--- a/Interannual_metrics_conversion.xlsx
+++ b/Interannual_metrics_conversion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noellepatterson/apps/Other/Climate_change_research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D331257-78A9-9A4B-9AB7-2E860FD92B19}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF9CA5D-5FD5-FB47-A749-0ED65EA63192}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="1640" windowWidth="15900" windowHeight="14700" xr2:uid="{ADBF414B-E432-A949-8C08-2739CE937D51}"/>
+    <workbookView xWindow="10280" yWindow="4940" windowWidth="15900" windowHeight="14700" xr2:uid="{ADBF414B-E432-A949-8C08-2739CE937D51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>fut-hist/hist</t>
   </si>
@@ -57,12 +57,6 @@
     <t>hist years in 20th/80th</t>
   </si>
   <si>
-    <t>RCP 4.5 avg</t>
-  </si>
-  <si>
-    <t>RCP 8.5 avg</t>
-  </si>
-  <si>
     <t>perc_20th</t>
   </si>
   <si>
@@ -82,6 +76,27 @@
   </si>
   <si>
     <t xml:space="preserve">Metric used in Geeta'a dataset. (Future # years - historic # years)/historic # years * 100, where number of years refers to number of years that are in the 20th or 80th percentile bins. </t>
+  </si>
+  <si>
+    <t>RCP 4.5 min</t>
+  </si>
+  <si>
+    <t>RCP 4.5 mean</t>
+  </si>
+  <si>
+    <t>RCP 4.5 max</t>
+  </si>
+  <si>
+    <t>RCP 8.5 min</t>
+  </si>
+  <si>
+    <t>RCP 8.5 mean</t>
+  </si>
+  <si>
+    <t>RCP 8.5 max</t>
+  </si>
+  <si>
+    <t>value in code (orig 80th)</t>
   </si>
 </sst>
 </file>
@@ -450,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE5235CA-CF63-654E-8AD3-425171C7E67C}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -472,7 +487,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -487,7 +502,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -507,14 +522,14 @@
         <v>-75.000000000000014</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G3">
-        <v>-3.3170000000000002</v>
+        <v>-39.06</v>
       </c>
       <c r="H3">
-        <f>G3/100*0.2+0.2</f>
-        <v>0.19336600000000001</v>
+        <f t="shared" ref="H3:H8" si="0">G3/100*0.2+0.2</f>
+        <v>0.12188</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -522,11 +537,11 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B18" si="0">A4*64</f>
+        <f t="shared" ref="B4:B18" si="1">A4*64</f>
         <v>4.8</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C18" si="1">64*0.2</f>
+        <f t="shared" ref="C4:C18" si="2">64*0.2</f>
         <v>12.8</v>
       </c>
       <c r="D4" s="1">
@@ -534,14 +549,14 @@
         <v>-62.5</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G4">
-        <v>-0.42099999999999949</v>
+        <v>-3.3170000000000002</v>
       </c>
       <c r="H4">
-        <f>G4/100*0.2+0.2</f>
-        <v>0.199158</v>
+        <f t="shared" si="0"/>
+        <v>0.19336600000000001</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -549,50 +564,80 @@
         <v>0.1</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.4</v>
       </c>
       <c r="C5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.8</v>
       </c>
       <c r="D5" s="1">
         <f>(B5-C5)/C5*100</f>
         <v>-50</v>
       </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5">
+        <v>32.6</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>0.26519999999999999</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6">
         <v>0.125</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="C6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.8</v>
       </c>
       <c r="D6" s="1">
         <f>(B6-C6)/C6*100</f>
         <v>-37.500000000000007</v>
       </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6">
+        <v>-54.76</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>9.0480000000000005E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7">
         <v>0.15</v>
       </c>
       <c r="B7">
+        <f t="shared" si="1"/>
+        <v>9.6</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="2"/>
+        <v>12.8</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" ref="D7:D18" si="3">(B7-C7)/C7*100</f>
+        <v>-25.000000000000007</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7">
+        <v>-0.42099999999999949</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="0"/>
-        <v>9.6</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="1"/>
-        <v>12.8</v>
-      </c>
-      <c r="D7" s="1">
-        <f t="shared" ref="D7:D18" si="2">(B7-C7)/C7*100</f>
-        <v>-25.000000000000007</v>
+        <v>0.199158</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -600,16 +645,26 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="B8">
+        <f t="shared" si="1"/>
+        <v>11.2</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="2"/>
+        <v>12.8</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="3"/>
+        <v>-12.500000000000011</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8">
+        <v>40.479999999999997</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="0"/>
-        <v>11.2</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="1"/>
-        <v>12.8</v>
-      </c>
-      <c r="D8" s="1">
-        <f t="shared" si="2"/>
-        <v>-12.500000000000011</v>
+        <v>0.28095999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -617,15 +672,15 @@
         <v>0.2</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.8</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.8</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -634,15 +689,15 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14.4</v>
       </c>
       <c r="C10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.8</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12.499999999999996</v>
       </c>
     </row>
@@ -651,15 +706,15 @@
         <v>0.25</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.8</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24.999999999999993</v>
       </c>
     </row>
@@ -668,15 +723,15 @@
         <v>0.27500000000000002</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.600000000000001</v>
       </c>
       <c r="C12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.8</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.500000000000007</v>
       </c>
     </row>
@@ -685,15 +740,15 @@
         <v>0.3</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19.2</v>
       </c>
       <c r="C13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.8</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>49.999999999999986</v>
       </c>
     </row>
@@ -702,11 +757,11 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20.8</v>
       </c>
       <c r="C14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.8</v>
       </c>
       <c r="D14" s="1">
@@ -719,15 +774,15 @@
         <v>0.35</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22.4</v>
       </c>
       <c r="C15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.8</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>74.999999999999972</v>
       </c>
     </row>
@@ -736,15 +791,15 @@
         <v>0.375</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="C16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.8</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>87.499999999999986</v>
       </c>
     </row>
@@ -753,15 +808,15 @@
         <v>0.4</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25.6</v>
       </c>
       <c r="C17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.8</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
     </row>
@@ -770,15 +825,15 @@
         <v>0.42499999999999999</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27.2</v>
       </c>
       <c r="C18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.8</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>112.49999999999997</v>
       </c>
     </row>
@@ -787,7 +842,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>4</v>
@@ -798,11 +853,14 @@
       <c r="D20" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="E20" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="G20" s="2" t="s">
         <v>0</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -821,15 +879,19 @@
         <f>(B21-C21)/C21*100</f>
         <v>-75.000000000000014</v>
       </c>
+      <c r="E21">
+        <f t="shared" ref="E21:E26" si="4">1-A21</f>
+        <v>0.95</v>
+      </c>
       <c r="F21" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G21">
-        <v>29.538999999999994</v>
+        <v>-47.8</v>
       </c>
       <c r="H21">
-        <f>G21/100*0.2+0.2</f>
-        <v>0.25907800000000003</v>
+        <f t="shared" ref="H21:H26" si="5">G21/100*0.2+0.2</f>
+        <v>0.10440000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -837,26 +899,30 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="B22">
-        <f t="shared" ref="B22:B36" si="3">A22*64</f>
+        <f t="shared" ref="B22:B36" si="6">A22*64</f>
         <v>4.8</v>
       </c>
       <c r="C22">
-        <f t="shared" ref="C22:C36" si="4">64*0.2</f>
+        <f t="shared" ref="C22:C36" si="7">64*0.2</f>
         <v>12.8</v>
       </c>
       <c r="D22" s="1">
         <f>(B22-C22)/C22*100</f>
         <v>-62.5</v>
       </c>
+      <c r="E22">
+        <f t="shared" si="4"/>
+        <v>0.92500000000000004</v>
+      </c>
       <c r="F22" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G22">
-        <v>53.21</v>
+        <v>29.54</v>
       </c>
       <c r="H22">
-        <f>G22/100*0.2+0.2</f>
-        <v>0.30642000000000003</v>
+        <f t="shared" si="5"/>
+        <v>0.25908000000000003</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -864,50 +930,92 @@
         <v>0.1</v>
       </c>
       <c r="B23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>6.4</v>
       </c>
       <c r="C23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>12.8</v>
       </c>
       <c r="D23" s="1">
         <f>(B23-C23)/C23*100</f>
         <v>-50</v>
       </c>
+      <c r="E23">
+        <f t="shared" si="4"/>
+        <v>0.9</v>
+      </c>
+      <c r="F23" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23">
+        <v>146.44999999999999</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="5"/>
+        <v>0.4929</v>
+      </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24">
         <v>0.125</v>
       </c>
       <c r="B24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="C24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>12.8</v>
       </c>
       <c r="D24" s="1">
         <f>(B24-C24)/C24*100</f>
         <v>-37.500000000000007</v>
       </c>
+      <c r="E24">
+        <f t="shared" si="4"/>
+        <v>0.875</v>
+      </c>
+      <c r="F24" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24">
+        <v>-54.19</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="5"/>
+        <v>9.1620000000000021E-2</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25">
         <v>0.15</v>
       </c>
       <c r="B25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>9.6</v>
       </c>
       <c r="C25">
+        <f t="shared" si="7"/>
+        <v>12.8</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" ref="D25:D31" si="8">(B25-C25)/C25*100</f>
+        <v>-25.000000000000007</v>
+      </c>
+      <c r="E25">
         <f t="shared" si="4"/>
-        <v>12.8</v>
-      </c>
-      <c r="D25" s="1">
-        <f t="shared" ref="D25:D31" si="5">(B25-C25)/C25*100</f>
-        <v>-25.000000000000007</v>
+        <v>0.85</v>
+      </c>
+      <c r="F25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25">
+        <v>53.21</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="5"/>
+        <v>0.30642000000000003</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -915,16 +1023,30 @@
         <v>0.17499999999999999</v>
       </c>
       <c r="B26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>11.2</v>
       </c>
       <c r="C26">
+        <f t="shared" si="7"/>
+        <v>12.8</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="8"/>
+        <v>-12.500000000000011</v>
+      </c>
+      <c r="E26">
         <f t="shared" si="4"/>
-        <v>12.8</v>
-      </c>
-      <c r="D26" s="1">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="F26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26">
+        <v>170.45</v>
+      </c>
+      <c r="H26">
         <f t="shared" si="5"/>
-        <v>-12.500000000000011</v>
+        <v>0.54089999999999994</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -932,16 +1054,20 @@
         <v>0.2</v>
       </c>
       <c r="B27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>12.8</v>
       </c>
       <c r="C27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>12.8</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
+      </c>
+      <c r="E27">
+        <f>1-A27</f>
+        <v>0.8</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -949,16 +1075,20 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="B28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>14.4</v>
       </c>
       <c r="C28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>12.8</v>
       </c>
       <c r="D28" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>12.499999999999996</v>
+      </c>
+      <c r="E28">
+        <f>1-A28</f>
+        <v>0.77500000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -966,16 +1096,20 @@
         <v>0.25</v>
       </c>
       <c r="B29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="C29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>12.8</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>24.999999999999993</v>
+      </c>
+      <c r="E29">
+        <f t="shared" ref="E29:E35" si="9">1-A29</f>
+        <v>0.75</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -983,16 +1117,20 @@
         <v>0.27500000000000002</v>
       </c>
       <c r="B30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>17.600000000000001</v>
       </c>
       <c r="C30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>12.8</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>37.500000000000007</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="9"/>
+        <v>0.72499999999999998</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1000,16 +1138,20 @@
         <v>0.3</v>
       </c>
       <c r="B31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>19.2</v>
       </c>
       <c r="C31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>12.8</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>49.999999999999986</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="9"/>
+        <v>0.7</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1017,116 +1159,136 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="B32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>20.8</v>
       </c>
       <c r="C32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>12.8</v>
       </c>
       <c r="D32" s="1">
         <f>(B32-C32)/C32*100</f>
         <v>62.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32">
+        <f t="shared" si="9"/>
+        <v>0.67500000000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>0.35</v>
       </c>
       <c r="B33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>22.4</v>
       </c>
       <c r="C33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>12.8</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" ref="D33:D36" si="6">(B33-C33)/C33*100</f>
+        <f t="shared" ref="D33:D36" si="10">(B33-C33)/C33*100</f>
         <v>74.999999999999972</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33">
+        <f t="shared" si="9"/>
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>0.375</v>
       </c>
       <c r="B34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="C34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>12.8</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>87.499999999999986</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34">
+        <f t="shared" si="9"/>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>0.4</v>
       </c>
       <c r="B35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>25.6</v>
       </c>
       <c r="C35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>12.8</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35">
+        <f t="shared" si="9"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>0.42499999999999999</v>
       </c>
       <c r="B36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>27.2</v>
       </c>
       <c r="C36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>12.8</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>112.49999999999997</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E36">
+        <f>1-A36</f>
+        <v>0.57499999999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix interannual metrics and add new plotting
</commit_message>
<xml_diff>
--- a/Interannual_metrics_conversion.xlsx
+++ b/Interannual_metrics_conversion.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noellepatterson/apps/Other/Climate_change_research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF9CA5D-5FD5-FB47-A749-0ED65EA63192}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25B8921-6D7B-3545-B741-FC96CDE657EB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10280" yWindow="4940" windowWidth="15900" windowHeight="14700" xr2:uid="{ADBF414B-E432-A949-8C08-2739CE937D51}"/>
+    <workbookView xWindow="5600" yWindow="480" windowWidth="18160" windowHeight="16200" activeTab="2" xr2:uid="{ADBF414B-E432-A949-8C08-2739CE937D51}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="first attempt" sheetId="1" r:id="rId1"/>
+    <sheet name="second attempt" sheetId="2" r:id="rId2"/>
+    <sheet name="tables" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="31">
   <si>
     <t>fut-hist/hist</t>
   </si>
@@ -97,6 +99,33 @@
   </si>
   <si>
     <t>value in code (orig 80th)</t>
+  </si>
+  <si>
+    <t>hist years in 20th (higher if getting drier)</t>
+  </si>
+  <si>
+    <t>max (0.2)</t>
+  </si>
+  <si>
+    <t>min (0.8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of years (out of 64 total) in historic data that are in 20th or 80th percentile bins. This will always be 20% + 20% of years by definition. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metric used in Geeta'a dataset. (Future # years - historic # years)/historic # years * 100, where number of years refers to number of years that are in the 20th or 80th percentile bins. I can't use this becasuse I don't have a before and after, I only have one dataset to start with. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noelle's metric which calculates the number of years in either 20th or 80th percentile bins divided by the total POR (64), in future scenario data. Ranges 0-1. 20th/80th percentile values calculated from historic data.* </t>
+  </si>
+  <si>
+    <t>* For Noelle's metric, 20th value will be 0-0.2, anything below 0.2 represen</t>
+  </si>
+  <si>
+    <t>value in code</t>
+  </si>
+  <si>
+    <t>val in code</t>
   </si>
 </sst>
 </file>
@@ -465,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE5235CA-CF63-654E-8AD3-425171C7E67C}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A41" sqref="A38:XFD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -498,6 +527,9 @@
       <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="G2" s="2" t="s">
         <v>0</v>
       </c>
@@ -880,8 +912,8 @@
         <v>-75.000000000000014</v>
       </c>
       <c r="E21">
-        <f t="shared" ref="E21:E26" si="4">1-A21</f>
-        <v>0.95</v>
+        <f t="shared" ref="E21:E26" si="4">A21+0.6</f>
+        <v>0.65</v>
       </c>
       <c r="F21" t="s">
         <v>15</v>
@@ -912,7 +944,7 @@
       </c>
       <c r="E22">
         <f t="shared" si="4"/>
-        <v>0.92500000000000004</v>
+        <v>0.67499999999999993</v>
       </c>
       <c r="F22" t="s">
         <v>16</v>
@@ -943,7 +975,7 @@
       </c>
       <c r="E23">
         <f t="shared" si="4"/>
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="F23" t="s">
         <v>17</v>
@@ -974,7 +1006,7 @@
       </c>
       <c r="E24">
         <f t="shared" si="4"/>
-        <v>0.875</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="F24" t="s">
         <v>18</v>
@@ -1005,7 +1037,7 @@
       </c>
       <c r="E25">
         <f t="shared" si="4"/>
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="F25" t="s">
         <v>19</v>
@@ -1036,7 +1068,7 @@
       </c>
       <c r="E26">
         <f t="shared" si="4"/>
-        <v>0.82499999999999996</v>
+        <v>0.77499999999999991</v>
       </c>
       <c r="F26" t="s">
         <v>20</v>
@@ -1054,7 +1086,7 @@
         <v>0.2</v>
       </c>
       <c r="B27">
-        <f t="shared" si="6"/>
+        <f>A27*64</f>
         <v>12.8</v>
       </c>
       <c r="C27">
@@ -1066,7 +1098,7 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <f>1-A27</f>
+        <f>A27+0.6</f>
         <v>0.8</v>
       </c>
     </row>
@@ -1083,12 +1115,12 @@
         <v>12.8</v>
       </c>
       <c r="D28" s="1">
-        <f t="shared" si="8"/>
+        <f>(B28-C28)/C28*100</f>
         <v>12.499999999999996</v>
       </c>
       <c r="E28">
-        <f>1-A28</f>
-        <v>0.77500000000000002</v>
+        <f t="shared" ref="E28:E36" si="9">A28+0.6</f>
+        <v>0.82499999999999996</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1108,8 +1140,8 @@
         <v>24.999999999999993</v>
       </c>
       <c r="E29">
-        <f t="shared" ref="E29:E35" si="9">1-A29</f>
-        <v>0.75</v>
+        <f t="shared" si="9"/>
+        <v>0.85</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1130,7 +1162,7 @@
       </c>
       <c r="E30">
         <f t="shared" si="9"/>
-        <v>0.72499999999999998</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1151,7 +1183,7 @@
       </c>
       <c r="E31">
         <f t="shared" si="9"/>
-        <v>0.7</v>
+        <v>0.89999999999999991</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1172,7 +1204,7 @@
       </c>
       <c r="E32">
         <f t="shared" si="9"/>
-        <v>0.67500000000000004</v>
+        <v>0.92500000000000004</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1188,12 +1220,12 @@
         <v>12.8</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" ref="D33:D36" si="10">(B33-C33)/C33*100</f>
+        <f t="shared" ref="D33:D35" si="10">(B33-C33)/C33*100</f>
         <v>74.999999999999972</v>
       </c>
       <c r="E33">
         <f t="shared" si="9"/>
-        <v>0.65</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1214,7 +1246,7 @@
       </c>
       <c r="E34">
         <f t="shared" si="9"/>
-        <v>0.625</v>
+        <v>0.97499999999999998</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1235,7 +1267,7 @@
       </c>
       <c r="E35">
         <f t="shared" si="9"/>
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1251,13 +1283,16 @@
         <v>12.8</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" si="10"/>
+        <f>(B36-C36)/C36*100</f>
         <v>112.49999999999997</v>
       </c>
       <c r="E36">
-        <f>1-A36</f>
-        <v>0.57499999999999996</v>
-      </c>
+        <f t="shared" si="9"/>
+        <v>1.0249999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="D37" s="1"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="2" t="s">
@@ -1289,6 +1324,2444 @@
       </c>
       <c r="B41" s="4" t="s">
         <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A294FD6-7831-AD48-9239-42422E14D8A6}">
+  <dimension ref="A1:I44"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3">
+        <v>0.05</v>
+      </c>
+      <c r="B3">
+        <f>64*0.2</f>
+        <v>12.8</v>
+      </c>
+      <c r="C3">
+        <f>A3*64</f>
+        <v>3.2</v>
+      </c>
+      <c r="D3" s="1">
+        <f>(B3-C3)/C3*100</f>
+        <v>300.00000000000006</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E7" si="0">0.2 + 0.2-A3</f>
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3">
+        <v>-39.06</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:C18" si="1">64*0.2</f>
+        <v>12.8</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C18" si="2">A4*64</f>
+        <v>4.8</v>
+      </c>
+      <c r="D4" s="1">
+        <f>(B4-C4)/C4*100</f>
+        <v>166.66666666666669</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4">
+        <v>-3.3170000000000002</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>0.1</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="1"/>
+        <v>12.8</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="2"/>
+        <v>6.4</v>
+      </c>
+      <c r="D5" s="1">
+        <f>(B5-C5)/C5*100</f>
+        <v>100</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5">
+        <v>32.6</v>
+      </c>
+      <c r="I5">
+        <v>0.249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>0.125</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="1"/>
+        <v>12.8</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D6" s="1">
+        <f>(B6-C6)/C6*100</f>
+        <v>60.000000000000007</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6">
+        <v>-54.76</v>
+      </c>
+      <c r="I6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>0.15</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>12.8</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="2"/>
+        <v>9.6</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" ref="D7:D18" si="3">(B7-C7)/C7*100</f>
+        <v>33.33333333333335</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7">
+        <v>-0.42099999999999949</v>
+      </c>
+      <c r="I7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>12.8</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="2"/>
+        <v>11.2</v>
+      </c>
+      <c r="D8" s="1">
+        <f>(B8-C8)/C8*100</f>
+        <v>14.285714285714299</v>
+      </c>
+      <c r="E8">
+        <f>0.2 + 0.2-A8</f>
+        <v>0.22500000000000003</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8">
+        <v>40.479999999999997</v>
+      </c>
+      <c r="I8">
+        <v>0.25800000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>0.2</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>12.8</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="2"/>
+        <v>12.8</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ref="E9:E18" si="4">0.2 + 0.2-A9</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>12.8</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="2"/>
+        <v>14.4</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="3"/>
+        <v>-11.111111111111107</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="4"/>
+        <v>0.17500000000000002</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>0.25</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>12.8</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="D11" s="1">
+        <f>(B11-C11)/C11*100</f>
+        <v>-19.999999999999996</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="4"/>
+        <v>0.15000000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>12.8</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="2"/>
+        <v>17.600000000000001</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="3"/>
+        <v>-27.272727272727277</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="4"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13">
+        <v>0.3</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>12.8</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="2"/>
+        <v>19.2</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="3"/>
+        <v>-33.333333333333329</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="4"/>
+        <v>0.10000000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>12.8</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="2"/>
+        <v>20.8</v>
+      </c>
+      <c r="D14" s="1">
+        <f>(B14-C14)/C14*100</f>
+        <v>-38.46153846153846</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="4"/>
+        <v>7.5000000000000011E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15">
+        <v>0.35</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>12.8</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="2"/>
+        <v>22.4</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="3"/>
+        <v>-42.857142857142847</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="4"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16">
+        <v>0.375</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>12.8</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="3"/>
+        <v>-46.666666666666664</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="4"/>
+        <v>2.5000000000000022E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>0.4</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>12.8</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="2"/>
+        <v>25.6</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="3"/>
+        <v>-50</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>12.8</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="2"/>
+        <v>27.2</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="3"/>
+        <v>-52.941176470588239</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="4"/>
+        <v>-2.4999999999999967E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <v>0.05</v>
+      </c>
+      <c r="B21">
+        <v>12.8</v>
+      </c>
+      <c r="C21">
+        <f>A21*64</f>
+        <v>3.2</v>
+      </c>
+      <c r="D21" s="1">
+        <f>(B21-C21)/C21*100</f>
+        <v>300.00000000000006</v>
+      </c>
+      <c r="E21">
+        <f>A21+0.6</f>
+        <v>0.65</v>
+      </c>
+      <c r="F21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21">
+        <v>-47.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="B22">
+        <v>12.8</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ref="C22:C36" si="5">A22*64</f>
+        <v>4.8</v>
+      </c>
+      <c r="D22" s="1">
+        <f>(B22-C22)/C22*100</f>
+        <v>166.66666666666669</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ref="E22:E36" si="6">A22+0.6</f>
+        <v>0.67499999999999993</v>
+      </c>
+      <c r="F22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22">
+        <v>29.54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
+        <v>0.1</v>
+      </c>
+      <c r="B23">
+        <v>12.8</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="5"/>
+        <v>6.4</v>
+      </c>
+      <c r="D23" s="1">
+        <f>(B23-C23)/C23*100</f>
+        <v>100</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="6"/>
+        <v>0.7</v>
+      </c>
+      <c r="F23" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23">
+        <v>146.44999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <v>0.125</v>
+      </c>
+      <c r="B24">
+        <v>12.8</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="D24" s="1">
+        <f>(B24-C24)/C24*100</f>
+        <v>60.000000000000007</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="6"/>
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="F24" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24">
+        <v>-54.19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>0.15</v>
+      </c>
+      <c r="B25">
+        <v>12.8</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="5"/>
+        <v>9.6</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" ref="D25:D31" si="7">(B25-C25)/C25*100</f>
+        <v>33.33333333333335</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="6"/>
+        <v>0.75</v>
+      </c>
+      <c r="F25" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25">
+        <v>53.21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="B26">
+        <v>12.8</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="5"/>
+        <v>11.2</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="7"/>
+        <v>14.285714285714299</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="6"/>
+        <v>0.77499999999999991</v>
+      </c>
+      <c r="F26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26">
+        <v>170.45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27">
+        <v>0.2</v>
+      </c>
+      <c r="B27">
+        <v>12.8</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="5"/>
+        <v>12.8</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="6"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="B28">
+        <v>12.8</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="5"/>
+        <v>14.4</v>
+      </c>
+      <c r="D28" s="1">
+        <f>(B28-C28)/C28*100</f>
+        <v>-11.111111111111107</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="6"/>
+        <v>0.82499999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29">
+        <v>0.25</v>
+      </c>
+      <c r="B29">
+        <v>12.8</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="7"/>
+        <v>-19.999999999999996</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="6"/>
+        <v>0.85</v>
+      </c>
+      <c r="F29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29">
+        <v>-47.8</v>
+      </c>
+      <c r="H29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="B30">
+        <v>12.8</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="5"/>
+        <v>17.600000000000001</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="7"/>
+        <v>-27.272727272727277</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="6"/>
+        <v>0.875</v>
+      </c>
+      <c r="F30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30">
+        <v>29.54</v>
+      </c>
+      <c r="H30">
+        <v>0.755</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
+        <v>0.3</v>
+      </c>
+      <c r="B31">
+        <v>12.8</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="5"/>
+        <v>19.2</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="7"/>
+        <v>-33.333333333333329</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="6"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="F31" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31">
+        <v>146.44999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="B32">
+        <v>12.8</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="5"/>
+        <v>20.8</v>
+      </c>
+      <c r="D32" s="1">
+        <f>(B32-C32)/C32*100</f>
+        <v>-38.46153846153846</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="6"/>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="F32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32">
+        <v>-54.19</v>
+      </c>
+      <c r="H32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33">
+        <v>0.35</v>
+      </c>
+      <c r="B33">
+        <v>12.8</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="5"/>
+        <v>22.4</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" ref="D33:D36" si="8">(B33-C33)/C33*100</f>
+        <v>-42.857142857142847</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="F33" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33">
+        <v>53.21</v>
+      </c>
+      <c r="H33">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34">
+        <v>0.375</v>
+      </c>
+      <c r="B34">
+        <v>12.8</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="8"/>
+        <v>-46.666666666666664</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="6"/>
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="F34" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34">
+        <v>170.45</v>
+      </c>
+      <c r="H34">
+        <v>0.67400000000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35">
+        <v>0.4</v>
+      </c>
+      <c r="B35">
+        <v>12.8</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="5"/>
+        <v>25.6</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="8"/>
+        <v>-50</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="B36">
+        <v>12.8</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="5"/>
+        <v>27.2</v>
+      </c>
+      <c r="D36" s="1">
+        <f>(B36-C36)/C36*100</f>
+        <v>-52.941176470588239</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="6"/>
+        <v>1.0249999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="B44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE58C654-A0AA-734A-83C7-51E61066EB04}">
+  <dimension ref="A1:K42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2">
+        <v>0.05</v>
+      </c>
+      <c r="H2">
+        <v>12.8</v>
+      </c>
+      <c r="I2">
+        <f>G2*64</f>
+        <v>3.2</v>
+      </c>
+      <c r="J2" s="1">
+        <f>(H2-I2)/I2*100</f>
+        <v>300.00000000000006</v>
+      </c>
+      <c r="K2">
+        <f>G2+0.6</f>
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>0.05</v>
+      </c>
+      <c r="B3">
+        <f>64*0.2</f>
+        <v>12.8</v>
+      </c>
+      <c r="C3">
+        <f>A3*64</f>
+        <v>3.2</v>
+      </c>
+      <c r="D3" s="1">
+        <f>(B3-C3)/C3*100</f>
+        <v>300.00000000000006</v>
+      </c>
+      <c r="E3">
+        <f>0.2 + 0.2-A3</f>
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="G3">
+        <v>5.5E-2</v>
+      </c>
+      <c r="H3">
+        <v>12.8</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I4" si="0">G3*64</f>
+        <v>3.52</v>
+      </c>
+      <c r="J3" s="1">
+        <f>(H3-I3)/I3*100</f>
+        <v>263.63636363636368</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K4" si="1">G3+0.6</f>
+        <v>0.65500000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>5.5E-2</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:C19" si="2">64*0.2</f>
+        <v>12.8</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C18" si="3">A4*64</f>
+        <v>3.52</v>
+      </c>
+      <c r="D4" s="1">
+        <f>(B4-C4)/C4*100</f>
+        <v>263.63636363636368</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E42" si="4">0.2 + 0.2-A4</f>
+        <v>0.34500000000000003</v>
+      </c>
+      <c r="G4">
+        <v>0.06</v>
+      </c>
+      <c r="H4">
+        <v>12.8</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>3.84</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" ref="J4:J30" si="5">(H4-I4)/I4*100</f>
+        <v>233.33333333333334</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>0.65999999999999992</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>0.06</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="2"/>
+        <v>12.8</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="3"/>
+        <v>3.84</v>
+      </c>
+      <c r="D5" s="1">
+        <f>(B5-C5)/C5*100</f>
+        <v>233.33333333333334</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="4"/>
+        <v>0.34</v>
+      </c>
+      <c r="G5">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="H5">
+        <v>12.8</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I30" si="6">G5*64</f>
+        <v>4.16</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="5"/>
+        <v>207.69230769230771</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ref="K5:K30" si="7">G5+0.6</f>
+        <v>0.66500000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="2"/>
+        <v>12.8</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="3"/>
+        <v>4.16</v>
+      </c>
+      <c r="D6" s="1">
+        <f>(B6-C6)/C6*100</f>
+        <v>207.69230769230771</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="4"/>
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H6">
+        <v>12.8</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="6"/>
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="5"/>
+        <v>185.71428571428569</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="7"/>
+        <v>0.66999999999999993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="2"/>
+        <v>12.8</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="3"/>
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" ref="D7:D18" si="8">(B7-C7)/C7*100</f>
+        <v>185.71428571428569</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="4"/>
+        <v>0.33</v>
+      </c>
+      <c r="G7">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="H7">
+        <v>12.8</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="6"/>
+        <v>4.7359999999999998</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="5"/>
+        <v>170.27027027027029</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="7"/>
+        <v>0.67399999999999993</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="2"/>
+        <v>12.8</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="3"/>
+        <v>4.8</v>
+      </c>
+      <c r="D8" s="1">
+        <f>(B8-C8)/C8*100</f>
+        <v>166.66666666666669</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="4"/>
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="G8">
+        <v>0.08</v>
+      </c>
+      <c r="H8">
+        <v>12.8</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="6"/>
+        <v>5.12</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="5"/>
+        <v>150</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="7"/>
+        <v>0.67999999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>0.08</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="2"/>
+        <v>12.8</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="3"/>
+        <v>5.12</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="8"/>
+        <v>150</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="4"/>
+        <v>0.32</v>
+      </c>
+      <c r="G9">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="H9">
+        <v>12.8</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="6"/>
+        <v>5.44</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="5"/>
+        <v>135.29411764705881</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="7"/>
+        <v>0.68499999999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="2"/>
+        <v>12.8</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="3"/>
+        <v>5.44</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="8"/>
+        <v>135.29411764705881</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="4"/>
+        <v>0.315</v>
+      </c>
+      <c r="G10">
+        <v>0.09</v>
+      </c>
+      <c r="H10">
+        <v>12.8</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="6"/>
+        <v>5.76</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="5"/>
+        <v>122.22222222222223</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="7"/>
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11">
+        <v>0.09</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="2"/>
+        <v>12.8</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="3"/>
+        <v>5.76</v>
+      </c>
+      <c r="D11" s="1">
+        <f>(B11-C11)/C11*100</f>
+        <v>122.22222222222223</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="4"/>
+        <v>0.31000000000000005</v>
+      </c>
+      <c r="G11">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="H11">
+        <v>12.8</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="6"/>
+        <v>6.08</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="5"/>
+        <v>110.5263157894737</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="7"/>
+        <v>0.69499999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="2"/>
+        <v>12.8</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="3"/>
+        <v>6.08</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="8"/>
+        <v>110.5263157894737</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="4"/>
+        <v>0.30500000000000005</v>
+      </c>
+      <c r="G12">
+        <v>0.1</v>
+      </c>
+      <c r="H12">
+        <v>12.8</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="6"/>
+        <v>6.4</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="7"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13">
+        <v>0.1</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="2"/>
+        <v>12.8</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="3"/>
+        <v>6.4</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="4"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="G13">
+        <v>0.105</v>
+      </c>
+      <c r="H13">
+        <v>12.8</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="6"/>
+        <v>6.72</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="5"/>
+        <v>90.476190476190496</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="7"/>
+        <v>0.70499999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14">
+        <v>0.105</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="2"/>
+        <v>12.8</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="3"/>
+        <v>6.72</v>
+      </c>
+      <c r="D14" s="1">
+        <f>(B14-C14)/C14*100</f>
+        <v>90.476190476190496</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="4"/>
+        <v>0.29500000000000004</v>
+      </c>
+      <c r="G14">
+        <v>0.11</v>
+      </c>
+      <c r="H14">
+        <v>12.8</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="6"/>
+        <v>7.04</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="5"/>
+        <v>81.818181818181827</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="7"/>
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15">
+        <v>0.11</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="2"/>
+        <v>12.8</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="3"/>
+        <v>7.04</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="8"/>
+        <v>81.818181818181827</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="4"/>
+        <v>0.29000000000000004</v>
+      </c>
+      <c r="G15">
+        <v>0.115</v>
+      </c>
+      <c r="H15">
+        <v>12.8</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="6"/>
+        <v>7.36</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" si="5"/>
+        <v>73.913043478260875</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="7"/>
+        <v>0.71499999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16">
+        <v>0.115</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="2"/>
+        <v>12.8</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="3"/>
+        <v>7.36</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="8"/>
+        <v>73.913043478260875</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="4"/>
+        <v>0.28500000000000003</v>
+      </c>
+      <c r="G16">
+        <v>0.12</v>
+      </c>
+      <c r="H16">
+        <v>12.8</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="6"/>
+        <v>7.68</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="5"/>
+        <v>66.666666666666686</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="7"/>
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17">
+        <v>0.12</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="2"/>
+        <v>12.8</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="3"/>
+        <v>7.68</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="8"/>
+        <v>66.666666666666686</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="4"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G17">
+        <v>0.125</v>
+      </c>
+      <c r="H17">
+        <v>12.8</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="5"/>
+        <v>60.000000000000007</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="7"/>
+        <v>0.72499999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18">
+        <v>0.125</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="2"/>
+        <v>12.8</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="8"/>
+        <v>60.000000000000007</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="4"/>
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="G18">
+        <v>0.13</v>
+      </c>
+      <c r="H18">
+        <v>12.8</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="6"/>
+        <v>8.32</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="5"/>
+        <v>53.846153846153854</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="7"/>
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19">
+        <v>0.13</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="2"/>
+        <v>12.8</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ref="C19:C24" si="9">A19*64</f>
+        <v>8.32</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" ref="D19:D24" si="10">(B19-C19)/C19*100</f>
+        <v>53.846153846153854</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="4"/>
+        <v>0.27</v>
+      </c>
+      <c r="G19">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="H19">
+        <v>12.8</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="6"/>
+        <v>8.64</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" si="5"/>
+        <v>48.148148148148145</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="7"/>
+        <v>0.73499999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ref="B20:B42" si="11">64*0.2</f>
+        <v>12.8</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="9"/>
+        <v>8.64</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="10"/>
+        <v>48.148148148148145</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="4"/>
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="G20">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H20">
+        <v>12.8</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="6"/>
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="5"/>
+        <v>42.857142857142847</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="7"/>
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="11"/>
+        <v>12.8</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="9"/>
+        <v>9.0879999999999992</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="10"/>
+        <v>40.84507042253523</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="4"/>
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="G21">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="H21">
+        <v>12.8</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="6"/>
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="J21" s="1">
+        <f t="shared" si="5"/>
+        <v>37.931034482758633</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="7"/>
+        <v>0.745</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="11"/>
+        <v>12.8</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="9"/>
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="10"/>
+        <v>37.931034482758633</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="4"/>
+        <v>0.255</v>
+      </c>
+      <c r="G22">
+        <v>0.15</v>
+      </c>
+      <c r="H22">
+        <v>12.8</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="6"/>
+        <v>9.6</v>
+      </c>
+      <c r="J22" s="1">
+        <f t="shared" si="5"/>
+        <v>33.33333333333335</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="7"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23">
+        <v>0.151</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="11"/>
+        <v>12.8</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="9"/>
+        <v>9.6639999999999997</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="10"/>
+        <v>32.450331125827823</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="4"/>
+        <v>0.24900000000000003</v>
+      </c>
+      <c r="G23">
+        <v>0.155</v>
+      </c>
+      <c r="H23">
+        <v>12.8</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="6"/>
+        <v>9.92</v>
+      </c>
+      <c r="J23" s="1">
+        <f t="shared" si="5"/>
+        <v>29.032258064516135</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="7"/>
+        <v>0.755</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24">
+        <v>0.155</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="11"/>
+        <v>12.8</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="9"/>
+        <v>9.92</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="10"/>
+        <v>29.032258064516135</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="4"/>
+        <v>0.24500000000000002</v>
+      </c>
+      <c r="G24">
+        <v>0.16</v>
+      </c>
+      <c r="H24">
+        <v>12.8</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="6"/>
+        <v>10.24</v>
+      </c>
+      <c r="J24" s="1">
+        <f t="shared" si="5"/>
+        <v>25.000000000000007</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="7"/>
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25">
+        <v>0.16</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="11"/>
+        <v>12.8</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ref="C25:C42" si="12">A25*64</f>
+        <v>10.24</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" ref="D25:D42" si="13">(B25-C25)/C25*100</f>
+        <v>25.000000000000007</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="4"/>
+        <v>0.24000000000000002</v>
+      </c>
+      <c r="G25">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="H25">
+        <v>12.8</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="6"/>
+        <v>10.56</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" si="5"/>
+        <v>21.212121212121211</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="7"/>
+        <v>0.76500000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="11"/>
+        <v>12.8</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="12"/>
+        <v>10.56</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="13"/>
+        <v>21.212121212121211</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="4"/>
+        <v>0.23500000000000001</v>
+      </c>
+      <c r="G26">
+        <v>0.17</v>
+      </c>
+      <c r="H26">
+        <v>12.8</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="6"/>
+        <v>10.88</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="5"/>
+        <v>17.647058823529409</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="7"/>
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27">
+        <v>0.17</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="11"/>
+        <v>12.8</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="12"/>
+        <v>10.88</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="13"/>
+        <v>17.647058823529409</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="4"/>
+        <v>0.23</v>
+      </c>
+      <c r="G27">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="H27">
+        <v>12.8</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="6"/>
+        <v>11.2</v>
+      </c>
+      <c r="J27" s="1">
+        <f t="shared" si="5"/>
+        <v>14.285714285714299</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="7"/>
+        <v>0.77499999999999991</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="11"/>
+        <v>12.8</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="12"/>
+        <v>11.2</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="13"/>
+        <v>14.285714285714299</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="4"/>
+        <v>0.22500000000000003</v>
+      </c>
+      <c r="G28">
+        <v>0.18</v>
+      </c>
+      <c r="H28">
+        <v>12.8</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="6"/>
+        <v>11.52</v>
+      </c>
+      <c r="J28" s="1">
+        <f t="shared" si="5"/>
+        <v>11.111111111111121</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="7"/>
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29">
+        <v>0.18</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="11"/>
+        <v>12.8</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="12"/>
+        <v>11.52</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="13"/>
+        <v>11.111111111111121</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="4"/>
+        <v>0.22000000000000003</v>
+      </c>
+      <c r="G29">
+        <v>0.185</v>
+      </c>
+      <c r="H29">
+        <v>12.8</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="6"/>
+        <v>11.84</v>
+      </c>
+      <c r="J29" s="1">
+        <f t="shared" si="5"/>
+        <v>8.1081081081081159</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="7"/>
+        <v>0.78499999999999992</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30">
+        <v>0.185</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="11"/>
+        <v>12.8</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="12"/>
+        <v>11.84</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="13"/>
+        <v>8.1081081081081159</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="4"/>
+        <v>0.21500000000000002</v>
+      </c>
+      <c r="G30">
+        <v>0.19</v>
+      </c>
+      <c r="H30">
+        <v>12.8</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="6"/>
+        <v>12.16</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" si="5"/>
+        <v>5.2631578947368469</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="7"/>
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31">
+        <v>0.19</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="11"/>
+        <v>12.8</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="12"/>
+        <v>12.16</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="13"/>
+        <v>5.2631578947368469</v>
+      </c>
+      <c r="E31">
+        <f>0.2 + 0.2-A31</f>
+        <v>0.21000000000000002</v>
+      </c>
+      <c r="G31">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="H31">
+        <v>12.8</v>
+      </c>
+      <c r="I31">
+        <f>G31*64</f>
+        <v>12.48</v>
+      </c>
+      <c r="J31" s="1">
+        <f>(H31-I31)/I31*100</f>
+        <v>2.5641025641025665</v>
+      </c>
+      <c r="K31">
+        <f>G31+0.6</f>
+        <v>0.79499999999999993</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="11"/>
+        <v>12.8</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="12"/>
+        <v>12.48</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="13"/>
+        <v>2.5641025641025665</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="4"/>
+        <v>0.20500000000000002</v>
+      </c>
+      <c r="G32">
+        <v>0.2</v>
+      </c>
+      <c r="H32">
+        <v>12.8</v>
+      </c>
+      <c r="I32">
+        <f t="shared" ref="I32:I36" si="14">G32*64</f>
+        <v>12.8</v>
+      </c>
+      <c r="J32" s="1">
+        <f>(H32-I32)/I32*100</f>
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <f t="shared" ref="K32:K36" si="15">G32+0.6</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33">
+        <v>0.2</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="11"/>
+        <v>12.8</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="12"/>
+        <v>12.8</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="4"/>
+        <v>0.2</v>
+      </c>
+      <c r="G33">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="H33">
+        <v>12.8</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="14"/>
+        <v>13.12</v>
+      </c>
+      <c r="J33" s="1">
+        <f t="shared" ref="J33:J36" si="16">(H33-I33)/I33*100</f>
+        <v>-2.4390243902438913</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="15"/>
+        <v>0.80499999999999994</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="11"/>
+        <v>12.8</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="12"/>
+        <v>13.12</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="13"/>
+        <v>-2.4390243902438913</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="4"/>
+        <v>0.19500000000000003</v>
+      </c>
+      <c r="G34">
+        <v>0.21</v>
+      </c>
+      <c r="H34">
+        <v>12.8</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="14"/>
+        <v>13.44</v>
+      </c>
+      <c r="J34" s="1">
+        <f t="shared" si="16"/>
+        <v>-4.761904761904753</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="15"/>
+        <v>0.80999999999999994</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35">
+        <v>0.21</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="11"/>
+        <v>12.8</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="12"/>
+        <v>13.44</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="13"/>
+        <v>-4.761904761904753</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="4"/>
+        <v>0.19000000000000003</v>
+      </c>
+      <c r="G35">
+        <v>0.215</v>
+      </c>
+      <c r="H35">
+        <v>12.8</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="14"/>
+        <v>13.76</v>
+      </c>
+      <c r="J35" s="1">
+        <f t="shared" si="16"/>
+        <v>-6.9767441860465045</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="15"/>
+        <v>0.81499999999999995</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36">
+        <v>0.215</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="11"/>
+        <v>12.8</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="12"/>
+        <v>13.76</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" si="13"/>
+        <v>-6.9767441860465045</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="4"/>
+        <v>0.18500000000000003</v>
+      </c>
+      <c r="G36">
+        <v>0.22</v>
+      </c>
+      <c r="H36">
+        <v>12.8</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="14"/>
+        <v>14.08</v>
+      </c>
+      <c r="J36" s="1">
+        <f t="shared" si="16"/>
+        <v>-9.0909090909090864</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="15"/>
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37">
+        <v>0.22</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="11"/>
+        <v>12.8</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="12"/>
+        <v>14.08</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="13"/>
+        <v>-9.0909090909090864</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="4"/>
+        <v>0.18000000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="11"/>
+        <v>12.8</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="12"/>
+        <v>14.4</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="13"/>
+        <v>-11.111111111111107</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="4"/>
+        <v>0.17500000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39">
+        <v>0.23</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="11"/>
+        <v>12.8</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="12"/>
+        <v>14.72</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="13"/>
+        <v>-13.043478260869565</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="4"/>
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="11"/>
+        <v>12.8</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="12"/>
+        <v>15.04</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="13"/>
+        <v>-14.893617021276587</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="4"/>
+        <v>0.16500000000000004</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41">
+        <v>0.24</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="11"/>
+        <v>12.8</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="12"/>
+        <v>15.36</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="13"/>
+        <v>-16.666666666666661</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="4"/>
+        <v>0.16000000000000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42">
+        <v>0.245</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="11"/>
+        <v>12.8</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="12"/>
+        <v>15.68</v>
+      </c>
+      <c r="D42" s="1">
+        <f t="shared" si="13"/>
+        <v>-18.367346938775501</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="4"/>
+        <v>0.15500000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>